<commit_message>
kalkulasi fe on download excel
</commit_message>
<xml_diff>
--- a/excels/Form 6 - Evaluasi Akhir.xlsx
+++ b/excels/Form 6 - Evaluasi Akhir.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/ecsms/excels/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFAB374-8DA2-8D47-A4FA-034C28E6A695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -144,7 +150,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -381,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -492,10 +498,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -512,6 +518,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -785,39 +794,39 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>37</v>
       </c>
@@ -831,7 +840,7 @@
       <c r="I4" s="36"/>
       <c r="J4" s="36"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -839,7 +848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -847,7 +856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -855,7 +864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -863,7 +872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="54" t="s">
         <v>6</v>
       </c>
@@ -881,7 +890,7 @@
       <c r="I11" s="54"/>
       <c r="J11" s="54"/>
     </row>
-    <row r="12" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -901,7 +910,7 @@
       <c r="I12" s="55"/>
       <c r="J12" s="55"/>
     </row>
-    <row r="13" spans="1:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -921,7 +930,7 @@
       <c r="I13" s="56"/>
       <c r="J13" s="56"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>10</v>
       </c>
@@ -943,7 +952,7 @@
       </c>
       <c r="J14" s="31"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>1</v>
       </c>
@@ -951,17 +960,17 @@
         <v>12</v>
       </c>
       <c r="C15" s="40"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
       <c r="F15" s="52">
         <v>0.2</v>
       </c>
       <c r="G15" s="52"/>
       <c r="H15" s="52"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>2</v>
       </c>
@@ -969,17 +978,17 @@
         <v>13</v>
       </c>
       <c r="C16" s="40"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
       <c r="F16" s="52">
         <v>0.3</v>
       </c>
       <c r="G16" s="52"/>
       <c r="H16" s="52"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>3</v>
       </c>
@@ -987,17 +996,17 @@
         <v>14</v>
       </c>
       <c r="C17" s="40"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="52">
         <v>0.35</v>
       </c>
       <c r="G17" s="52"/>
       <c r="H17" s="52"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>4</v>
       </c>
@@ -1005,17 +1014,17 @@
         <v>15</v>
       </c>
       <c r="C18" s="40"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
       <c r="F18" s="52">
         <v>0.15</v>
       </c>
       <c r="G18" s="52"/>
       <c r="H18" s="52"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="40" t="s">
         <v>16</v>
       </c>
@@ -1026,10 +1035,13 @@
       <c r="F19" s="40"/>
       <c r="G19" s="40"/>
       <c r="H19" s="40"/>
-      <c r="I19" s="41"/>
+      <c r="I19" s="53">
+        <f>SUM(I15:I18)</f>
+        <v>0</v>
+      </c>
       <c r="J19" s="41"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>17</v>
       </c>
@@ -1047,7 +1059,7 @@
       </c>
       <c r="J20" s="45"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1059,7 +1071,7 @@
       <c r="I21" s="46"/>
       <c r="J21" s="47"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>18</v>
       </c>
@@ -1077,7 +1089,7 @@
       </c>
       <c r="J22" s="49"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -1093,7 +1105,7 @@
       </c>
       <c r="J23" s="51"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>19</v>
       </c>
@@ -1109,7 +1121,7 @@
       <c r="I24" s="34"/>
       <c r="J24" s="35"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>20</v>
       </c>
@@ -1129,7 +1141,7 @@
       <c r="I25" s="38"/>
       <c r="J25" s="39"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>21</v>
       </c>
@@ -1149,7 +1161,7 @@
       <c r="I26" s="38"/>
       <c r="J26" s="39"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>23</v>
       </c>
@@ -1169,7 +1181,7 @@
       <c r="I27" s="38"/>
       <c r="J27" s="39"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
         <v>24</v>
       </c>
@@ -1189,7 +1201,7 @@
       <c r="I28" s="28"/>
       <c r="J28" s="29"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1201,7 +1213,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="16"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -1269,6 +1281,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3">JDHWM6R55FRK-3-1098</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3">
+      <Url>http://intra-ecorr.pertamina.com:1043/sites/DIR/_layouts/DocIdRedir.aspx?ID=JDHWM6R55FRK-3-1098</Url>
+      <Description>JDHWM6R55FRK-3-1098</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3398B66F6FF2D41BB4BC1F9AFA58185" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a6c582f2b0bd71f194a9173d25feba3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bbc7d0c2066ec31eb77a1a91b3421a26" ns2:_="">
     <xsd:import namespace="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3"/>
@@ -1413,7 +1437,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1459,7 +1483,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1468,30 +1492,46 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3">JDHWM6R55FRK-3-1098</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3">
-      <Url>http://intra-ecorr.pertamina.com:1043/sites/DIR/_layouts/DocIdRedir.aspx?ID=JDHWM6R55FRK-3-1098</Url>
-      <Description>JDHWM6R55FRK-3-1098</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51C9F6B4-3161-4CA9-AFBD-5F82185E13D1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B2E6BC-8ECE-4CEE-B2A7-0C2AB748E678}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69225441-566D-40C5-A927-397853997736}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51C9F6B4-3161-4CA9-AFBD-5F82185E13D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f8ce19fc-6d1c-4a32-9ccc-c9d52d339ce3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{350BFC04-F163-4318-B394-B2E204502345}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69225441-566D-40C5-A927-397853997736}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B2E6BC-8ECE-4CEE-B2A7-0C2AB748E678}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{350BFC04-F163-4318-B394-B2E204502345}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>